<commit_message>
feat: DATA and GENERATION
</commit_message>
<xml_diff>
--- a/results-data/analysis.xlsx
+++ b/results-data/analysis.xlsx
@@ -1,30 +1,120 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrateur\Documents\Master\Advanced algorithms\moha\knapsackProblem\results-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6B90EE-8D1A-4857-B46F-BAA0508892F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ou" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Hello</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.8e-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.005272</t>
+  </si>
+  <si>
+    <t>0.0005381059646606445</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.00014335999999999998</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0053094399999999995</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>0.004988193511962891</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.001584</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.006808</t>
+  </si>
+  <si>
+    <t>0.0007777309417724609</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.00011276000000000002</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0053027199999999995</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7.599999999999999e-05</t>
+  </si>
+  <si>
+    <t>0.0019943714141845703</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.00017199999999999998</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0053679999999999995</t>
+  </si>
+  <si>
+    <t>0.0007979631423950196</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8.56e-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.005281599999999999</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -40,7 +130,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -48,23 +138,972 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ou!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ou!$A$2:$A$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ou!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.3810596466064399E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.7773094177245995E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9796314239501901E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C0E3-415C-B1D3-42C9BC140968}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1862398592"/>
+        <c:axId val="1862406496"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1862398592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1100"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1862406496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1862406496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1862398592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1614487</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Graphique 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DF17EE8-BD07-03D9-4A82-5C3DDC1CCB62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B4F38673-157F-4319-AAD8-7F46E402921A}" name="Tableau2" displayName="Tableau2" ref="A1:B10" totalsRowShown="0">
+  <autoFilter ref="A1:B10" xr:uid="{B4F38673-157F-4319-AAD8-7F46E402921A}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{7CF49AC7-1CB8-4F5F-9B34-0257B466A520}" name="x"/>
+    <tableColumn id="2" xr3:uid="{A0E567F4-5571-4985-94DF-B0E1D772A2CF}" name="y"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -106,7 +1145,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -138,9 +1177,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -172,6 +1229,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -347,34 +1422,166 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="41" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1">
-        <v>1234</v>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1234.56</v>
+        <v>10</v>
+      </c>
+      <c r="B2" s="4">
+        <v>5.3810596466064399E-4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3" s="4">
+        <v>7.7773094177245995E-4</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1000</v>
+      </c>
+      <c r="B4" s="4">
+        <v>7.9796314239501901E-4</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="b">
-        <v>1</v>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D7" s="2"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>